<commit_message>
MockUp y BackLog Actualizados
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Ciclo 4\repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25E1978D-9114-4FDE-A59D-A188B8C51182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B75A29E-2287-4716-81B2-DA1F08C8FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Identificador de historia</t>
   </si>
@@ -75,12 +75,6 @@
 Para: Tener ubicación del cliente</t>
   </si>
   <si>
-    <t>Historia: Recibir mensaje del cliente
-Como: Administrador de la app
-Quiero: recibir una señal cuando el cliente tenga una solicitud
-Para: Recoger lo que el cliente necesita entregar</t>
-  </si>
-  <si>
     <t>Historia: Registrarme en la app
 Como: Usuario
 Quiero: registrarme en la base de datos de clientes
@@ -117,9 +111,6 @@
 Para: Ingresar a la app</t>
   </si>
   <si>
-    <t>Activity con formulario de registro varios Edit Text dependiendo cuantos datos se solicitaran y boton para enviar informacion</t>
-  </si>
-  <si>
     <t>Activity con formulario de registro varios Edit Text dependiendo cuantos datos se ingresaran y boton para enviar informacion</t>
   </si>
   <si>
@@ -135,16 +126,10 @@
     <t>Activity con 2 Edit Text uno para el usuario otro para la contraseña y 2 botones uno para ingresar y otro para registrarse si es un usuario nuevo Boton recuperar contraseña</t>
   </si>
   <si>
-    <t>Detallar datos</t>
-  </si>
-  <si>
     <t>Elementos de la interfaz</t>
   </si>
   <si>
     <t>Activity que despliega google maps se seleciona punto en el mapa y envía coordenadas o dirección a la base de datos con un boton</t>
-  </si>
-  <si>
-    <t>Activity con boton de solicitar servicio</t>
   </si>
   <si>
     <t>Historia: Recibir solicitud del cliente
@@ -154,6 +139,27 @@
   </si>
   <si>
     <t>Activity con un recycler view donde muestra listado de clientes con solicitudes</t>
+  </si>
+  <si>
+    <t>Los botones son de color azul y los edit text fondo blanco y la color de la letra negra</t>
+  </si>
+  <si>
+    <t>Se solicitara Nombre, Apellido, Sexo, correo electrónico, número de identificación, nombre del negocio, fecha de nacimiento, dirección del negocio</t>
+  </si>
+  <si>
+    <t>La cantidad de recycler view dependen del número de solicitudes recibidas</t>
+  </si>
+  <si>
+    <t>Historia: Recibir y responder mensaje del cliente
+Como: Usuario / Administrador de la app
+Quiero: recibir un mensaje del cliente
+Para: Comunicarme con el cliente</t>
+  </si>
+  <si>
+    <t>Activity con formulario de registro con 8 Edit Text y Text View para ingresar los datos y boton de colo azúl para enviar informacion, 1 TextView que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
+  </si>
+  <si>
+    <t>Activity con 1 TextView donde se le solicita que en el EditText especifique tipo de carga y peso, 1 EditText para que escriba lo solicitado, un boton de solicitar servicio, 1 TextView con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
   </si>
 </sst>
 </file>
@@ -191,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -228,10 +234,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -243,10 +249,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -258,13 +264,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -276,11 +325,100 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -289,46 +427,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,51 +811,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D934AE-131A-4196-878A-37C45723C87B}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.77734375" customWidth="1"/>
-    <col min="7" max="7" width="33.44140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" style="7"/>
+    <col min="2" max="2" width="54.77734375" style="7" customWidth="1"/>
+    <col min="3" max="6" width="11.5546875" style="7"/>
+    <col min="7" max="7" width="33.44140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="7"/>
+    <col min="9" max="9" width="21" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="10" t="s">
+      <c r="G1" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -703,213 +872,227 @@
       <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="9">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="20"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="5">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D10" s="13">
         <v>3</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4">
-        <v>3</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="4">
-        <v>3</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se actualizo backlog y mockup
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Ciclo 4\repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B75A29E-2287-4716-81B2-DA1F08C8FB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0653BA-4621-4290-B36C-1963575EDF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -812,7 +812,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
se deja un solo backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Ciclo 4\repositorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0653BA-4621-4290-B36C-1963575EDF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F89C64F-EE01-4DDD-8979-61ECE3FDDE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Identificador de historia</t>
   </si>
@@ -156,17 +156,50 @@
 Para: Comunicarme con el cliente</t>
   </si>
   <si>
-    <t>Activity con formulario de registro con 8 Edit Text y Text View para ingresar los datos y boton de colo azúl para enviar informacion, 1 TextView que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
-  </si>
-  <si>
-    <t>Activity con 1 TextView donde se le solicita que en el EditText especifique tipo de carga y peso, 1 EditText para que escriba lo solicitado, un boton de solicitar servicio, 1 TextView con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
+    <t>Activity con formulario de registro con 8 Edit Text y Text View para ingresar los datos y boton de colo azúl para enviar informacion, 1 Toast que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
+  </si>
+  <si>
+    <t>Activity con 1 TextView donde se le solicita que en el EditText especifique tipo de carga y peso, 1 EditText para que escriba lo solicitado, un boton de solicitar servicio, 1 Alert Dialoge con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
+  </si>
+  <si>
+    <t>No se realizara como activity es una función que realiza el admin directamente en la bas de datos</t>
+  </si>
+  <si>
+    <t>Botón que envia a una actividad dónde se busca la ubicación en google maps</t>
+  </si>
+  <si>
+    <t>Un botón y el mapa de google</t>
+  </si>
+  <si>
+    <t>muestra mensaje enviados y recibidos</t>
+  </si>
+  <si>
+    <t>Edit Text para escribir mensaje y un botón para enviar</t>
+  </si>
+  <si>
+    <t>Historia: Olvido contraseña
+Como: Usuario
+Quiero: Recibir correo electrónico con link para reactivar contraseña
+Para: Ingresar a la App</t>
+  </si>
+  <si>
+    <t>Activity con 1 EditText donde usuario escribe correo electrónico para enviar link de reactivación y boton enviar</t>
+  </si>
+  <si>
+    <t>Historia: Detalle de la solicitud
+Como: Administrador
+Quiero: Revisar detalle de la solicitud del cliente
+Para: Tener la información para realizar la entrega</t>
+  </si>
+  <si>
+    <t>Activity con 11 TextView donde muestra el detalle de la solicitud realizada por el cliente Nombre, Apellido, Sexo, correo electrónico, número de identificación, nombre del negocio, fecha de nacimiento, dirección del negocio, tipo de carga y peso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +215,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +234,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -221,62 +265,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -359,9 +347,20 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -370,7 +369,33 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -379,55 +404,76 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -435,59 +481,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -811,280 +875,318 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D934AE-131A-4196-878A-37C45723C87B}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="7"/>
-    <col min="2" max="2" width="54.77734375" style="7" customWidth="1"/>
-    <col min="3" max="6" width="11.5546875" style="7"/>
-    <col min="7" max="7" width="33.44140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="7"/>
-    <col min="9" max="9" width="21" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="7"/>
+    <col min="1" max="1" width="11.5546875" style="4"/>
+    <col min="2" max="2" width="54.77734375" style="4" customWidth="1"/>
+    <col min="3" max="6" width="11.5546875" style="4"/>
+    <col min="7" max="7" width="35.109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="20">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="22">
+        <v>2</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D4" s="13">
         <v>3</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="E4" s="13"/>
+      <c r="F4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="19"/>
+      <c r="H4" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="24"/>
     </row>
-    <row r="3" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
+    <row r="5" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D5" s="3">
         <v>3</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5" t="s">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="22"/>
+      <c r="H5" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5" t="s">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="10"/>
+      <c r="H6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="5" t="s">
+    <row r="7" spans="1:9" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D7" s="27">
         <v>2</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5">
-        <v>2</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="22">
         <v>3</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="E8" s="22"/>
+      <c r="F8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="10" t="s">
+      <c r="H8" s="22"/>
+      <c r="I8" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>3</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="10"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+    <row r="10" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="3">
         <v>3</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+    <row r="11" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+    <row r="12" spans="1:9" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="9">
+        <v>3</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -1096,6 +1198,9 @@
       <c r="H13" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
se actualiza backlog se crean layout activity login y registro
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\Ciclo 4\repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\AndroidStudioProjects\AppMovil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4D8E039-6E25-4484-A5B7-73CCD6832915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED4894-11E0-422A-985A-BEF33D7BFFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -144,9 +144,6 @@
     <t>Los botones son de color azul y los edit text fondo blanco y la color de la letra negra</t>
   </si>
   <si>
-    <t>Se solicitara Nombre, Apellido, Sexo, correo electrónico, número de identificación, nombre del negocio, fecha de nacimiento, dirección del negocio</t>
-  </si>
-  <si>
     <t>La cantidad de recycler view dependen del número de solicitudes recibidas</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
 Para: Comunicarme con el cliente</t>
   </si>
   <si>
-    <t>Activity con formulario de registro con 8 Edit Text y Text View para ingresar los datos y boton de colo azúl para enviar informacion, 1 Toast que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
-  </si>
-  <si>
     <t>Activity con 1 TextView donde se le solicita que en el EditText especifique tipo de carga y peso, 1 EditText para que escriba lo solicitado, un boton de solicitar servicio, 1 Alert Dialoge con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
   </si>
   <si>
@@ -193,6 +187,12 @@
   </si>
   <si>
     <t>Activity con 11 TextView donde muestra el detalle de la solicitud realizada por el cliente Nombre, Apellido, Sexo, correo electrónico, número de identificación, nombre del negocio, fecha de nacimiento, dirección del negocio, tipo de carga y peso</t>
+  </si>
+  <si>
+    <t>Se solicitara Nombre, Apellido, Sexo, correo electrónico, número de identificación, nombre del negocio, fecha de nacimiento, dirección del negocio, usuario y contraseña y repita constraseña</t>
+  </si>
+  <si>
+    <t>Activity con formulario de registro con 11 Edit Text con hint para ingresar los datos y boton de colo azúl para enviar informacion, 1 Toast que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
   </si>
 </sst>
 </file>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D934AE-131A-4196-878A-37C45723C87B}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,7 +944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -962,11 +962,11 @@
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="6" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -990,7 +990,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I4" s="24"/>
     </row>
@@ -1015,10 +1015,10 @@
         <v>24</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1026,7 +1026,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>8</v>
@@ -1042,10 +1042,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1066,7 +1066,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H7" s="27"/>
       <c r="I7" s="28"/>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1147,7 +1147,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -1160,7 +1160,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="6"/>
@@ -1170,7 +1170,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -1183,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>

</xml_diff>

<commit_message>
nuevos layouts y actualiza backlog
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\AndroidStudioProjects\AppMovil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EED4894-11E0-422A-985A-BEF33D7BFFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B92C2-694A-456B-A50B-38E1A6F49DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>Identificador de historia</t>
   </si>
@@ -153,9 +153,6 @@
 Para: Comunicarme con el cliente</t>
   </si>
   <si>
-    <t>Activity con 1 TextView donde se le solicita que en el EditText especifique tipo de carga y peso, 1 EditText para que escriba lo solicitado, un boton de solicitar servicio, 1 Alert Dialoge con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
-  </si>
-  <si>
     <t>No se realizara como activity es una función que realiza el admin directamente en la bas de datos</t>
   </si>
   <si>
@@ -193,6 +190,18 @@
   </si>
   <si>
     <t>Activity con formulario de registro con 11 Edit Text con hint para ingresar los datos y boton de colo azúl para enviar informacion, 1 Toast que diga "usuario registrado satisfactoriamente, Bienvenido"</t>
+  </si>
+  <si>
+    <t>Layout OK</t>
+  </si>
+  <si>
+    <t>Pendiente Toast</t>
+  </si>
+  <si>
+    <t>Activity con 1 EditText donde se le solicita que en el  especifique tipo de carga y peso, un boton de solicitar servicio, 1 Alert Dialoge con mensaje que diga "Solicitud recibida su paquete será recogido el día de mañana"</t>
+  </si>
+  <si>
+    <t>Pendiente Alert Dialoge</t>
   </si>
 </sst>
 </file>
@@ -876,7 +885,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,7 +948,9 @@
       <c r="G2" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="22" t="s">
+        <v>41</v>
+      </c>
       <c r="I2" s="23" t="s">
         <v>27</v>
       </c>
@@ -962,11 +973,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="I3" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -990,7 +1003,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="24"/>
     </row>
@@ -1015,10 +1028,10 @@
         <v>24</v>
       </c>
       <c r="H5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>32</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1042,13 +1055,13 @@
         <v>19</v>
       </c>
       <c r="H6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="7" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="119.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="25">
         <v>6</v>
       </c>
@@ -1066,9 +1079,11 @@
         <v>9</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="27"/>
+        <v>43</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>44</v>
+      </c>
       <c r="I7" s="28"/>
     </row>
     <row r="8" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
@@ -1147,7 +1162,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -1160,9 +1175,11 @@
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="I11" s="6"/>
     </row>
     <row r="12" spans="1:9" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -1170,7 +1187,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -1183,9 +1200,11 @@
         <v>9</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
se actualiza backlog, layout home admin y buttons para cambiar de activity
</commit_message>
<xml_diff>
--- a/BackLog.xlsx
+++ b/BackLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\AndroidStudioProjects\AppMovil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B92C2-694A-456B-A50B-38E1A6F49DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E2B74E-AFEB-4661-A8DA-3E0935923CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2AF7358-79BA-4F9E-9C53-1E454E621E33}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
   <si>
     <t>Identificador de historia</t>
   </si>
@@ -162,12 +162,6 @@
     <t>Un botón y el mapa de google</t>
   </si>
   <si>
-    <t>muestra mensaje enviados y recibidos</t>
-  </si>
-  <si>
-    <t>Edit Text para escribir mensaje y un botón para enviar</t>
-  </si>
-  <si>
     <t>Historia: Olvido contraseña
 Como: Usuario
 Quiero: Recibir correo electrónico con link para reactivar contraseña
@@ -202,6 +196,12 @@
   </si>
   <si>
     <t>Pendiente Alert Dialoge</t>
+  </si>
+  <si>
+    <t>Activity con enlace directo al whatsapp del proveedor</t>
+  </si>
+  <si>
+    <t>3 Text View con dirección nombre y telefono del proveedor , logo de whatsapp que redirecciona a la app para chatear</t>
   </si>
 </sst>
 </file>
@@ -884,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D934AE-131A-4196-878A-37C45723C87B}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -949,7 +949,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I2" s="23" t="s">
         <v>27</v>
@@ -973,13 +973,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="I3" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
@@ -1034,7 +1034,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1049,16 +1049,16 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="119.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1079,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H7" s="27" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I7" s="28"/>
     </row>
@@ -1106,7 +1106,9 @@
       <c r="G8" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="22" t="s">
+        <v>39</v>
+      </c>
       <c r="I8" s="23" t="s">
         <v>28</v>
       </c>
@@ -1162,7 +1164,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -1175,10 +1177,10 @@
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I11" s="6"/>
     </row>
@@ -1187,7 +1189,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>8</v>
@@ -1200,10 +1202,10 @@
         <v>9</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I12" s="10"/>
     </row>

</xml_diff>